<commit_message>
'add full SD setup to server'
</commit_message>
<xml_diff>
--- a/sample_files/Input_SD.xlsx
+++ b/sample_files/Input_SD.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
   <si>
     <t>Targeting type</t>
   </si>
@@ -98,13 +98,16 @@
     <t>CONTEXTUAL CPC</t>
   </si>
   <si>
-    <t>PAGE VISITS or CVR</t>
+    <t>PAGE VISITS</t>
   </si>
   <si>
     <t>AUDIENCE CPC</t>
   </si>
   <si>
     <t>T00030</t>
+  </si>
+  <si>
+    <t>CVR</t>
   </si>
   <si>
     <t>category="166164011"</t>
@@ -117,9 +120,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d.m"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -199,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -210,9 +211,6 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -222,7 +220,7 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
@@ -232,16 +230,13 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -551,34 +546,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -621,7 +616,7 @@
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
@@ -641,245 +636,245 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33">
-      <c r="A2" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="44.25">
+      <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="5">
         <v>20221212</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="5">
         <v>1</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="5">
         <v>15</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="8">
-        <v>44686</v>
-      </c>
-      <c r="O2" s="5" t="s">
+      <c r="N2" s="7">
+        <v>5.5</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33">
-      <c r="A3" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="44.25">
+      <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <v>20221212</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <v>1</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <v>15</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="8">
-        <v>44686</v>
-      </c>
-      <c r="O3" s="5" t="s">
+      <c r="N3" s="7">
+        <v>7.6</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="5"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="30">
-      <c r="A4" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="31.5">
+      <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="5" t="s">
+      <c r="G4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>20221212</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>1</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>15</v>
       </c>
-      <c r="M4" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" s="8">
-        <v>44686</v>
-      </c>
-      <c r="O4" s="5" t="s">
+      <c r="M4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="5">
+        <v>20</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="5"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="30">
-      <c r="A5" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="31.5">
+      <c r="A5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="5">
+        <v>20221212</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="5">
+        <v>1</v>
+      </c>
+      <c r="L5" s="5">
+        <v>15</v>
+      </c>
+      <c r="M5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="6">
-        <v>20221212</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="6">
-        <v>1</v>
-      </c>
-      <c r="L5" s="6">
-        <v>15</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="N5" s="8">
-        <v>44686</v>
-      </c>
-      <c r="O5" s="5" t="s">
+      <c r="N5" s="5">
+        <v>90</v>
+      </c>
+      <c r="O5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>